<commit_message>
Sector coupled implemented correctly
</commit_message>
<xml_diff>
--- a/test/configs/data/components_backup.xlsx
+++ b/test/configs/data/components_backup.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="7824" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Carrier" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="61">
   <si>
     <t>solar</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>batterylink 1-2</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -857,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -934,7 +937,7 @@
         <v>41</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>50</v>
@@ -964,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,7 +1028,7 @@
         <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -1037,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1056,7 +1059,7 @@
         <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -1065,16 +1068,16 @@
         <v>1</v>
       </c>
       <c r="H3" s="1">
-        <v>0.95</v>
+        <v>0.5</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="K3" s="1">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>